<commit_message>
Add MSA definitions to bullet list (#649)
</commit_message>
<xml_diff>
--- a/app/static/media/documents/Requirements_Brief_Template.xlsx
+++ b/app/static/media/documents/Requirements_Brief_Template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Matison\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcome" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="140">
   <si>
     <t>Question</t>
   </si>
@@ -456,18 +451,6 @@
     <t>Create a title for your brief</t>
   </si>
   <si>
-    <t>For example 'Developer needed for immediate start'. Or simply, 'Ethical Hacker—6 month project'.
-You can update it later if needed.
-Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What type of digital specialist do you need?
-</t>
-  </si>
-  <si>
-    <t>Choose one option.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Where will the work take place?
 </t>
   </si>
@@ -537,15 +520,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Contracts cannot exceed 12 months.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All specialists in the Digital Marketplace have already agreed to the terms and conditions in the Deed of Standing Offer.
-However, if you need to set out any additional terms and conditions, you can do so here.
-</t>
-  </si>
-  <si>
     <t>How much can you spend per day?</t>
   </si>
   <si>
@@ -564,10 +538,6 @@
   </si>
   <si>
     <t>Maximum number of specialists you’ll evaluate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We recommend that you evaluate at least 3 specialists.
-</t>
   </si>
   <si>
     <t>Evaluation weighting
@@ -619,14 +589,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Set technical competence criteria
-Technical competence is how well the seller can do the work you need them to do.
-Evaluate specialists’ technical competence using criteria for:
-- essential skills and experience
-- nice-to-have skills and experience
-</t>
-  </si>
-  <si>
     <t>Up to 20 criteria, 300 characters per criteria</t>
   </si>
   <si>
@@ -643,15 +605,6 @@
 - Work as a team with our organisation and other sellers
 - Transparent and collaborative when making decisions
 - Have a no-blame culture and encourage people to learn from their mistakes</t>
-  </si>
-  <si>
-    <t>How you’ll assess the specialists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You must ask all specialists that reach the assessment stage for a work history.
-Choose additional ways to assess specialists.
-You can only use the methods you choose here, for example if you don’t select an interview, you won’t be able to interview specialists.
-</t>
   </si>
   <si>
     <t xml:space="preserve">How long your requirements will be open for </t>
@@ -684,51 +637,13 @@
     <t>Question and answer session details</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Highlight one of the thirteen options below.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
-Agile Coach
-Helps individuals, teams and managers be as effective as possible by embedding an agile culture.
-Business Analyst
-Analyses a service or organisation’s business processes and systems. Specifies, collects and presents findings.
-Delivery Manager
-Enables agile teams to deliver high-quality services by removing obstacles or blockers to progress and facilitating project meetings.
-Developer
-Builds quality, well-tested software and sites according to standards and best practice.
-Digital Transformation Adviser
-Digital Transformation Advisers provide leadership in delivering new programs of work in state, territory and federal government agencies, or across multiple functions.
-Ethical Hacker
-Ensures system security, identifies cyber security risks, applies risk treatments, detects and manages cyber security incidents.
-Inclusive Designer
-Supports the team with an in-depth knowledge of best practice in accessible development.
-Interaction Designer
-Responsible for designing a user-focused and accessible service, and making use of established design patterns.
-Performance and Web Analyst
-Specifies, collects and presents the key performance data and analysis for their service.
-Product Manager
-Works with the team to create the vision for the product, and sets the day-to-day priorities to fulfil that vision and ensure the team delivers.
-Service Designer
-Designs user-focused services that meet web standards and contributes to the development and continual enhancement of products.
-Technical Lead/Architect
-The most senior technical person in the team. Their role is to break down complex problems and lead by example in writing quality code.
-User Researcher
-Helps the team develop a deep understanding of their users and user needs.
- Web Operations Engineer (Web Devops)
-Runs the production systems, helps the team deploy quickly and reliably and ensures the smooth running of the service.</t>
-    </r>
+    <t>Essential skills and experience
+List all the specific skills or experience the specialist must have, for example have experience designing services for users with low digital literacy.</t>
+  </si>
+  <si>
+    <t>Nice-to-have skills and experience
+If too many specialists have all the essential skills and experience, use the nice-to-have skills and experience to exclude specialists.
+List the skills and experience you’d like the specialist to have, for example "provide evidence of delivering at scale."</t>
   </si>
   <si>
     <r>
@@ -738,9 +653,25 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Highlight all that will apply. Work History is mandatory
-Work history 
-A work history can give you a view of a specialist’s skills and experience.
+      <t xml:space="preserve">Highlight one of the eleven options below.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(definitions for each option can be found at https://marketplace1.zendesk.com/hc/en-gb/articles/115011271567-What-you-can-buy)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -750,7 +681,71 @@
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">
-References 
+- Strategy and Policy 
+- User research and Design 
+- Agile delivery and Governance 
+- Software engineering and Development 
+- Support and Operations 
+- Content and Publishing 
+- Change, Training and Transformation
+- Marketing, Communications and Engagement 
+- Cyber security 
+- Data science and management 
+- Emerging technologies 
+</t>
+    </r>
+  </si>
+  <si>
+    <t>For example 'Developer needed for immediate start'. Or simply, 'Ethical Hacker—6 month project'.
+You can update it later if needed.</t>
+  </si>
+  <si>
+    <t>All sellers that respond to your brief in the Digital Marketplace have agreed to the terms and conditions in the Master Agreement.
+There will be times when the nature of your opportunity means you may need to add to or amend the default positions of the Master Agreement. If you need to, you can set out any additional terms and conditions here.</t>
+  </si>
+  <si>
+    <t>Area of expertise</t>
+  </si>
+  <si>
+    <t>Choose the primary area of expertise needed to complete the tasks in your brief. 
+Sellers must be approved in this area of expertise before they are eligible to apply for your brief. Sellers who are not yet approved for this area can request assessment while the brief is open on the Marketplace, and if approved will be eligible to apply.</t>
+  </si>
+  <si>
+    <t>We recommend that you evaluate at least 3 specialists.
+After shortlisting all responses, this is the number of specialists you'll evaluate in detail.</t>
+  </si>
+  <si>
+    <t>Evaluation criteria 
+When a seller applies for your brief they’ll provide a written response to each of your essential and desirable criteria. Clearly stating the skills and experience you need here will make your evaluation easier later. 
+Remember, when evaluating consider all relevant financial and non-financial costs and benefits including: 
+- the quality of the goods and services
+- fitness for purpose of the proposal
+- the seller’s experience and performance history
+- flexibility of the proposal, including innovation and adaptability over the lifecycle of the procurement
+- environmental sustainability of the proposed goods and services, such as energy efficiency and environmental impact
+- whole-of-life costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How will you verify the specialist is right for the role? </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Highlight all that will apply. Resumes are mandatory
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">References 
 References are a good way of confirming whether a specialist has done the work they’ve said they’ve done. You should always ask for references that relate to a specific timeframe, for example work they’ve done in the last 2 years.
 Interview 
 An interview can help you understand whether a specialist or team has the skills needed to work on your project. It will also help you see whether they will be a good fit for your existing team. You should follow an agreed format in which you ask all specialists the same set of questions.
@@ -764,19 +759,74 @@
     </r>
   </si>
   <si>
-    <t>Essential skills and experience
-List all the specific skills or experience the specialist must have, for example have experience designing services for users with low digital literacy.</t>
+    <t xml:space="preserve">You must review the resumes of all specialists who reach the evaluation stage.
+You can only use the methods you choose here, for example if you don’t select an interview, you won’t be able to interview specialists.
+</t>
   </si>
   <si>
-    <t>Nice-to-have skills and experience
-If too many specialists have all the essential skills and experience, use the nice-to-have skills and experience to exclude specialists.
-List the skills and experience you’d like the specialist to have, for example "provide evidence of delivering at scale."</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>While the application period is open, you need to reply to all questions sellers ask about your requirements.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+When a seller asks a question, you’ll be sent an email to the email address you registered with.
+You’ll need to post all questions and answers on the Digital Marketplace so that all sellers can see them.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Providing a question and answer session is optional but it means you can explain your needs and answer any questions quickly.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+You must include:
+- the type of session you want to run, eg webinar, phone conference or meeting
+- the date and time of the session (this should happen within 1 week of publishing your requirements)
+Depending on the type of session you choose, you could also include:
+- software needed
+- the url
+- the phone number
+- the access code
+- the address (including postcode)
+- anything else needed to take part
+This information will only be available to eligible sellers who have logged in.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If you select Open to select or Open to one, you are required to manually add the selected seller's email addresses.
+If specifying sellers, they must be registered on the Digital Marketplace at the time of publishing or they will not be able to respond. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -902,7 +952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -935,9 +985,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -959,20 +1006,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1016,24 +1049,11 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1044,6 +1064,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1236,7 +1283,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>273050</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>5073650</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1285,7 +1332,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>273050</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>5073650</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1339,7 +1386,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>273050</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>5073650</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1681,10 +1728,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1713,7 +1762,7 @@
       <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="31"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1741,15 +1790,15 @@
       <c r="AF1" s="1"/>
     </row>
     <row r="2" spans="1:32" ht="12.5">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1777,19 +1826,19 @@
       <c r="AF2" s="2"/>
     </row>
     <row r="3" spans="1:32" ht="62.5">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="35" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="28" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="30"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1817,19 +1866,19 @@
       <c r="AF3" s="2"/>
     </row>
     <row r="4" spans="1:32" ht="125">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="32"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -1857,19 +1906,19 @@
       <c r="AF4" s="2"/>
     </row>
     <row r="5" spans="1:32" ht="50">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="29"/>
+      <c r="E5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="30"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1897,19 +1946,19 @@
       <c r="AF5" s="2"/>
     </row>
     <row r="6" spans="1:32" ht="87.5">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="35" t="s">
+      <c r="D6" s="29"/>
+      <c r="E6" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="30"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1937,19 +1986,19 @@
       <c r="AF6" s="2"/>
     </row>
     <row r="7" spans="1:32" ht="50">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="35" t="s">
+      <c r="D7" s="29"/>
+      <c r="E7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1977,19 +2026,19 @@
       <c r="AF7" s="2"/>
     </row>
     <row r="8" spans="1:32" ht="125">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="35" t="s">
+      <c r="D8" s="29"/>
+      <c r="E8" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="30"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2017,23 +2066,23 @@
       <c r="AF8" s="2"/>
     </row>
     <row r="9" spans="1:32" ht="62.5">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="30"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2061,19 +2110,19 @@
       <c r="AF9" s="2"/>
     </row>
     <row r="10" spans="1:32" ht="300">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -2101,19 +2150,19 @@
       <c r="AF10" s="2"/>
     </row>
     <row r="11" spans="1:32" ht="50">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="35" t="s">
+      <c r="D11" s="29"/>
+      <c r="E11" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="30"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -2141,21 +2190,21 @@
       <c r="AF11" s="2"/>
     </row>
     <row r="12" spans="1:32" ht="13">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="30"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -2183,21 +2232,21 @@
       <c r="AF12" s="2"/>
     </row>
     <row r="13" spans="1:32" ht="50">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="35" t="s">
+      <c r="D13" s="29"/>
+      <c r="E13" s="28" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -2225,21 +2274,21 @@
       <c r="AF13" s="2"/>
     </row>
     <row r="14" spans="1:32" ht="75">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="35" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2267,23 +2316,23 @@
       <c r="AF14" s="2"/>
     </row>
     <row r="15" spans="1:32" ht="87.5">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2311,19 +2360,19 @@
       <c r="AF15" s="2"/>
     </row>
     <row r="16" spans="1:32" ht="50">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
       <c r="F16" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2351,21 +2400,21 @@
       <c r="AF16" s="2"/>
     </row>
     <row r="17" spans="1:32" ht="26">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34" t="s">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="36"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -2393,23 +2442,23 @@
       <c r="AF17" s="2"/>
     </row>
     <row r="18" spans="1:32" ht="100">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="31" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="30"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2437,23 +2486,23 @@
       <c r="AF18" s="2"/>
     </row>
     <row r="19" spans="1:32" ht="125">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="30"/>
+      <c r="G19" s="23"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2481,19 +2530,19 @@
       <c r="AF19" s="2"/>
     </row>
     <row r="20" spans="1:32" ht="50">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39" t="s">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="35" t="s">
+      <c r="D20" s="29"/>
+      <c r="E20" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="30"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2521,15 +2570,15 @@
       <c r="AF20" s="2"/>
     </row>
     <row r="21" spans="1:32" ht="13">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="30"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2557,17 +2606,17 @@
       <c r="AF21" s="2"/>
     </row>
     <row r="22" spans="1:32" ht="39">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40" t="s">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="30"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2595,17 +2644,17 @@
       <c r="AF22" s="2"/>
     </row>
     <row r="23" spans="1:32" ht="13">
-      <c r="A23" s="42"/>
-      <c r="B23" s="43" t="s">
+      <c r="A23" s="35"/>
+      <c r="B23" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="33"/>
+      <c r="G23" s="26"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -2633,19 +2682,19 @@
       <c r="AF23" s="5"/>
     </row>
     <row r="24" spans="1:32" ht="137.5">
-      <c r="A24" s="42"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="35" t="s">
+      <c r="A24" s="35"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="28" t="s">
         <v>64</v>
       </c>
       <c r="F24" s="11"/>
-      <c r="G24" s="33"/>
+      <c r="G24" s="26"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -2673,19 +2722,19 @@
       <c r="AF24" s="5"/>
     </row>
     <row r="25" spans="1:32" ht="75">
-      <c r="A25" s="42"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="35" t="s">
+      <c r="A25" s="35"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="37" t="s">
         <v>66</v>
       </c>
       <c r="F25" s="11"/>
-      <c r="G25" s="33"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -2713,19 +2762,19 @@
       <c r="AF25" s="5"/>
     </row>
     <row r="26" spans="1:32" ht="37.5">
-      <c r="A26" s="42"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="34" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="E26" s="37" t="s">
         <v>68</v>
       </c>
       <c r="F26" s="11"/>
-      <c r="G26" s="33"/>
+      <c r="G26" s="26"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -2753,17 +2802,17 @@
       <c r="AF26" s="5"/>
     </row>
     <row r="27" spans="1:32" ht="13" customHeight="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="48" t="s">
+      <c r="A27" s="27"/>
+      <c r="B27" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="33"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="26"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -2791,19 +2840,19 @@
       <c r="AF27" s="5"/>
     </row>
     <row r="28" spans="1:32" ht="225">
-      <c r="A28" s="34"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="35" t="s">
-        <v>137</v>
+      <c r="A28" s="27"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="28" t="s">
+        <v>126</v>
       </c>
-      <c r="D28" s="50"/>
-      <c r="E28" s="35" t="s">
+      <c r="D28" s="38"/>
+      <c r="E28" s="28" t="s">
         <v>71</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="33"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -2831,19 +2880,19 @@
       <c r="AF28" s="5"/>
     </row>
     <row r="29" spans="1:32" ht="100">
-      <c r="A29" s="34"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="35" t="s">
-        <v>138</v>
+      <c r="A29" s="27"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="28" t="s">
+        <v>127</v>
       </c>
-      <c r="D29" s="50" t="s">
+      <c r="D29" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="28" t="s">
         <v>71</v>
       </c>
       <c r="F29" s="11"/>
-      <c r="G29" s="33"/>
+      <c r="G29" s="26"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -2871,17 +2920,17 @@
       <c r="AF29" s="5"/>
     </row>
     <row r="30" spans="1:32" ht="137.5">
-      <c r="A30" s="34"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="35" t="s">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="14" t="s">
+      <c r="D30" s="38"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G30" s="33"/>
+      <c r="G30" s="26"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -2909,21 +2958,21 @@
       <c r="AF30" s="5"/>
     </row>
     <row r="31" spans="1:32" ht="100">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34" t="s">
+      <c r="A31" s="27"/>
+      <c r="B31" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="50"/>
-      <c r="E31" s="35" t="s">
+      <c r="D31" s="38"/>
+      <c r="E31" s="28" t="s">
         <v>71</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G31" s="33"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -2951,19 +3000,19 @@
       <c r="AF31" s="5"/>
     </row>
     <row r="32" spans="1:32" ht="262.5">
-      <c r="A32" s="40"/>
-      <c r="B32" s="40" t="s">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
       <c r="F32" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G32" s="30"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -2991,21 +3040,21 @@
       <c r="AF32" s="2"/>
     </row>
     <row r="33" spans="1:32" ht="255" customHeight="1">
-      <c r="A33" s="40"/>
-      <c r="B33" s="40" t="s">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="41" t="s">
+      <c r="D33" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="36"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="G33" s="30"/>
+      <c r="G33" s="23"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="3"/>
@@ -3033,15 +3082,15 @@
       <c r="AF33" s="2"/>
     </row>
     <row r="34" spans="1:32" ht="12.5">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="30"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="23"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -3069,17 +3118,17 @@
       <c r="AF34" s="2"/>
     </row>
     <row r="35" spans="1:32" ht="37.5">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40" t="s">
+      <c r="A35" s="33"/>
+      <c r="B35" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="30"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -3107,23 +3156,23 @@
       <c r="AF35" s="2"/>
     </row>
     <row r="36" spans="1:32" ht="387.5">
-      <c r="A36" s="40"/>
-      <c r="B36" s="40" t="s">
+      <c r="A36" s="33"/>
+      <c r="B36" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="41" t="s">
+      <c r="D36" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E36" s="41" t="s">
+      <c r="E36" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="51" t="s">
+      <c r="F36" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="G36" s="30"/>
+      <c r="G36" s="23"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -3151,19 +3200,19 @@
       <c r="AF36" s="2"/>
     </row>
     <row r="37" spans="1:32" ht="138">
-      <c r="A37" s="36"/>
-      <c r="B37" s="52" t="s">
+      <c r="A37" s="29"/>
+      <c r="B37" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="14" t="s">
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="30"/>
+      <c r="G37" s="23"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -3191,13 +3240,13 @@
       <c r="AF37" s="2"/>
     </row>
     <row r="38" spans="1:32" ht="12.5">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -36085,23 +36134,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8" style="54" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" style="54" customWidth="1"/>
-    <col min="3" max="3" width="56.54296875" style="54" customWidth="1"/>
-    <col min="4" max="5" width="11.08984375" style="54" customWidth="1"/>
-    <col min="6" max="6" width="70" style="54" customWidth="1"/>
-    <col min="7" max="7" width="5.26953125" style="54" customWidth="1"/>
-    <col min="8" max="16384" width="14.453125" style="54"/>
+    <col min="1" max="1" width="8" style="42" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" style="42" customWidth="1"/>
+    <col min="3" max="3" width="56.54296875" style="42" customWidth="1"/>
+    <col min="4" max="5" width="11.08984375" style="42" customWidth="1"/>
+    <col min="6" max="6" width="82.81640625" style="42" customWidth="1"/>
+    <col min="7" max="7" width="5.26953125" style="42" customWidth="1"/>
+    <col min="8" max="16384" width="14.453125" style="42"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13">
@@ -36121,210 +36170,210 @@
       <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="53"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:7" ht="12.5">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="53"/>
-    </row>
-    <row r="3" spans="1:7" ht="75">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="41"/>
+    </row>
+    <row r="3" spans="1:7" ht="50">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22" t="s">
         <v>94</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="53"/>
-    </row>
-    <row r="4" spans="1:7" ht="409.5">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23" t="s">
-        <v>96</v>
+      <c r="G3" s="41"/>
+    </row>
+    <row r="4" spans="1:7" ht="125">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="10" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
-      <c r="G4" s="53"/>
-    </row>
-    <row r="5" spans="1:7" ht="125">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23" t="s">
+      <c r="G4" s="41"/>
+    </row>
+    <row r="5" spans="1:7" ht="62.5">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22" t="s">
         <v>98</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>99</v>
       </c>
       <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="10" t="s">
+      <c r="E5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="41"/>
+    </row>
+    <row r="6" spans="1:7" ht="87.5">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="G5" s="53"/>
-    </row>
-    <row r="6" spans="1:7" ht="62.5">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23" t="s">
+      <c r="C6" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="53"/>
-    </row>
-    <row r="7" spans="1:7" ht="87.5">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23" t="s">
-        <v>103</v>
+      <c r="G6" s="41"/>
+    </row>
+    <row r="7" spans="1:7" ht="26">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="53"/>
+      <c r="G7" s="41"/>
     </row>
     <row r="8" spans="1:7" ht="26">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="41"/>
+    </row>
+    <row r="9" spans="1:7" ht="50">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="53"/>
-    </row>
-    <row r="9" spans="1:7" ht="26">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="F9" s="9"/>
-      <c r="G9" s="53"/>
-    </row>
-    <row r="10" spans="1:7" ht="50">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23" t="s">
-        <v>107</v>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:7" ht="87.5">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="53"/>
+      <c r="G10" s="41"/>
     </row>
     <row r="11" spans="1:7" ht="87.5">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23" t="s">
-        <v>35</v>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="41"/>
+    </row>
+    <row r="12" spans="1:7" ht="37.5">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7" t="s">
-        <v>16</v>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="41"/>
+    </row>
+    <row r="13" spans="1:7" ht="39">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22" t="s">
+        <v>45</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="53"/>
-    </row>
-    <row r="12" spans="1:7" ht="87.5">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="53"/>
-    </row>
-    <row r="13" spans="1:7" ht="37.5">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D13" s="8"/>
       <c r="E13" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="53"/>
-    </row>
-    <row r="14" spans="1:7" ht="39">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23" t="s">
-        <v>45</v>
+      <c r="G13" s="41"/>
+    </row>
+    <row r="14" spans="1:7" ht="87.5">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="F14" s="9"/>
-      <c r="G14" s="53"/>
-    </row>
-    <row r="15" spans="1:7" ht="87.5">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23" t="s">
-        <v>48</v>
+      <c r="G14" s="41"/>
+    </row>
+    <row r="15" spans="1:7" ht="75">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22" t="s">
+        <v>110</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>2</v>
@@ -36333,227 +36382,225 @@
         <v>33</v>
       </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="53"/>
-    </row>
-    <row r="16" spans="1:7" ht="75">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23" t="s">
-        <v>115</v>
+      <c r="G15" s="41"/>
+    </row>
+    <row r="16" spans="1:7" ht="87.5">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="D16" s="8"/>
       <c r="E16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="53"/>
-    </row>
-    <row r="17" spans="1:31" ht="87.5">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="53"/>
-    </row>
-    <row r="18" spans="1:31" ht="13">
-      <c r="A18" s="26" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="41"/>
+    </row>
+    <row r="17" spans="1:31" ht="13">
+      <c r="A17" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="53"/>
-    </row>
-    <row r="19" spans="1:31" ht="39">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23" t="s">
-        <v>119</v>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="41"/>
+    </row>
+    <row r="18" spans="1:31" ht="200.5">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" s="41"/>
+    </row>
+    <row r="19" spans="1:31" ht="50">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="53"/>
+      <c r="G19" s="41"/>
     </row>
     <row r="20" spans="1:31" ht="100.5">
-      <c r="A20" s="22"/>
-      <c r="B20" s="28" t="s">
-        <v>121</v>
+      <c r="A20" s="21"/>
+      <c r="B20" s="54" t="s">
+        <v>115</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
-      <c r="T20" s="56"/>
-      <c r="U20" s="56"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="56"/>
-      <c r="Y20" s="56"/>
-      <c r="Z20" s="56"/>
-      <c r="AA20" s="56"/>
-      <c r="AB20" s="56"/>
-      <c r="AC20" s="56"/>
-      <c r="AD20" s="56"/>
-      <c r="AE20" s="56"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="44"/>
+      <c r="Q20" s="44"/>
+      <c r="R20" s="44"/>
+      <c r="S20" s="44"/>
+      <c r="T20" s="44"/>
+      <c r="U20" s="44"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="44"/>
+      <c r="X20" s="44"/>
+      <c r="Y20" s="44"/>
+      <c r="Z20" s="44"/>
+      <c r="AA20" s="44"/>
+      <c r="AB20" s="44"/>
+      <c r="AC20" s="44"/>
+      <c r="AD20" s="44"/>
+      <c r="AE20" s="44"/>
     </row>
     <row r="21" spans="1:31" ht="50.5">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F21" s="11"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="56"/>
-      <c r="U21" s="56"/>
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
-      <c r="Y21" s="56"/>
-      <c r="Z21" s="56"/>
-      <c r="AA21" s="56"/>
-      <c r="AB21" s="56"/>
-      <c r="AC21" s="56"/>
-      <c r="AD21" s="56"/>
-      <c r="AE21" s="56"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="44"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="44"/>
+      <c r="X21" s="44"/>
+      <c r="Y21" s="44"/>
+      <c r="Z21" s="44"/>
+      <c r="AA21" s="44"/>
+      <c r="AB21" s="44"/>
+      <c r="AC21" s="44"/>
+      <c r="AD21" s="44"/>
+      <c r="AE21" s="44"/>
     </row>
     <row r="22" spans="1:31" ht="13">
-      <c r="A22" s="22"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="23" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="22" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F22" s="11"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="56"/>
-      <c r="S22" s="56"/>
-      <c r="T22" s="56"/>
-      <c r="U22" s="56"/>
-      <c r="V22" s="56"/>
-      <c r="W22" s="56"/>
-      <c r="X22" s="56"/>
-      <c r="Y22" s="56"/>
-      <c r="Z22" s="56"/>
-      <c r="AA22" s="56"/>
-      <c r="AB22" s="56"/>
-      <c r="AC22" s="56"/>
-      <c r="AD22" s="56"/>
-      <c r="AE22" s="56"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="44"/>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="44"/>
+      <c r="S22" s="44"/>
+      <c r="T22" s="44"/>
+      <c r="U22" s="44"/>
+      <c r="V22" s="44"/>
+      <c r="W22" s="44"/>
+      <c r="X22" s="44"/>
+      <c r="Y22" s="44"/>
+      <c r="Z22" s="44"/>
+      <c r="AA22" s="44"/>
+      <c r="AB22" s="44"/>
+      <c r="AC22" s="44"/>
+      <c r="AD22" s="44"/>
+      <c r="AE22" s="44"/>
     </row>
     <row r="23" spans="1:31" ht="184.5" customHeight="1">
-      <c r="A23" s="23"/>
-      <c r="B23" s="29" t="s">
-        <v>125</v>
+      <c r="A23" s="22"/>
+      <c r="B23" s="55" t="s">
+        <v>134</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="56"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="56"/>
-      <c r="U23" s="56"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="56"/>
-      <c r="Y23" s="56"/>
-      <c r="Z23" s="56"/>
-      <c r="AA23" s="56"/>
-      <c r="AB23" s="56"/>
-      <c r="AC23" s="56"/>
-      <c r="AD23" s="56"/>
-      <c r="AE23" s="56"/>
-    </row>
-    <row r="24" spans="1:31" ht="92.25" customHeight="1">
-      <c r="A24" s="23"/>
-      <c r="B24" s="25"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44"/>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="44"/>
+      <c r="U23" s="44"/>
+      <c r="V23" s="44"/>
+      <c r="W23" s="44"/>
+      <c r="X23" s="44"/>
+      <c r="Y23" s="44"/>
+      <c r="Z23" s="44"/>
+      <c r="AA23" s="44"/>
+      <c r="AB23" s="44"/>
+      <c r="AC23" s="44"/>
+      <c r="AD23" s="44"/>
+      <c r="AE23" s="44"/>
+    </row>
+    <row r="24" spans="1:31" ht="217.5" customHeight="1">
+      <c r="A24" s="22"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="7" t="s">
         <v>73</v>
       </c>
@@ -36561,40 +36608,40 @@
         <v>2</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
-      <c r="F24" s="13" t="s">
-        <v>127</v>
+      <c r="F24" s="10" t="s">
+        <v>120</v>
       </c>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="56"/>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="56"/>
-      <c r="S24" s="56"/>
-      <c r="T24" s="56"/>
-      <c r="U24" s="56"/>
-      <c r="V24" s="56"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="56"/>
-      <c r="Y24" s="56"/>
-      <c r="Z24" s="56"/>
-      <c r="AA24" s="56"/>
-      <c r="AB24" s="56"/>
-      <c r="AC24" s="56"/>
-      <c r="AD24" s="56"/>
-      <c r="AE24" s="56"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="44"/>
+      <c r="U24" s="44"/>
+      <c r="V24" s="44"/>
+      <c r="W24" s="44"/>
+      <c r="X24" s="44"/>
+      <c r="Y24" s="44"/>
+      <c r="Z24" s="44"/>
+      <c r="AA24" s="44"/>
+      <c r="AB24" s="44"/>
+      <c r="AC24" s="44"/>
+      <c r="AD24" s="44"/>
+      <c r="AE24" s="44"/>
     </row>
     <row r="25" spans="1:31" ht="99.75" customHeight="1">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23" t="s">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -36602,128 +36649,129 @@
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>128</v>
+      <c r="F25" s="13" t="s">
+        <v>121</v>
       </c>
-      <c r="G25" s="55"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="56"/>
-      <c r="S25" s="56"/>
-      <c r="T25" s="56"/>
-      <c r="U25" s="56"/>
-      <c r="V25" s="56"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="56"/>
-      <c r="Y25" s="56"/>
-      <c r="Z25" s="56"/>
-      <c r="AA25" s="56"/>
-      <c r="AB25" s="56"/>
-      <c r="AC25" s="56"/>
-      <c r="AD25" s="56"/>
-      <c r="AE25" s="56"/>
-    </row>
-    <row r="26" spans="1:31" ht="377">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15" t="s">
-        <v>129</v>
+      <c r="G25" s="43"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="44"/>
+      <c r="S25" s="44"/>
+      <c r="T25" s="44"/>
+      <c r="U25" s="44"/>
+      <c r="V25" s="44"/>
+      <c r="W25" s="44"/>
+      <c r="X25" s="44"/>
+      <c r="Y25" s="44"/>
+      <c r="Z25" s="44"/>
+      <c r="AA25" s="44"/>
+      <c r="AB25" s="44"/>
+      <c r="AC25" s="44"/>
+      <c r="AD25" s="44"/>
+      <c r="AE25" s="44"/>
+    </row>
+    <row r="26" spans="1:31" ht="326">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14" t="s">
+        <v>135</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>130</v>
+      <c r="C26" s="15" t="s">
+        <v>137</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="G26" s="53"/>
+      <c r="G26" s="41"/>
     </row>
     <row r="27" spans="1:31" ht="12.5">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="53"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="41"/>
     </row>
     <row r="28" spans="1:31" ht="51">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15" t="s">
-        <v>131</v>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14" t="s">
+        <v>122</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>132</v>
+      <c r="C28" s="15" t="s">
+        <v>123</v>
       </c>
-      <c r="D28" s="16"/>
+      <c r="D28" s="15"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="14" t="s">
-        <v>133</v>
+      <c r="F28" s="13" t="s">
+        <v>124</v>
       </c>
-      <c r="G28" s="53"/>
-    </row>
-    <row r="29" spans="1:31" ht="375">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15" t="s">
-        <v>134</v>
+      <c r="G28" s="41"/>
+    </row>
+    <row r="29" spans="1:31" ht="365">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14" t="s">
+        <v>125</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>89</v>
+      <c r="C29" s="15" t="s">
+        <v>138</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="53"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="41"/>
     </row>
     <row r="30" spans="1:31" ht="137.5">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20" t="s">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="10" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
-      <c r="G30" s="53"/>
+      <c r="G30" s="41"/>
     </row>
     <row r="31" spans="1:31" ht="12.5">
-      <c r="A31" s="53"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A27:F27"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>